<commit_message>
update xuat hoa don
</commit_message>
<xml_diff>
--- a/src/Report/HoaDon.xlsx
+++ b/src/Report/HoaDon.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BTLJava\quanliduan\src\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9415174-A44D-43F8-9DD2-EDE20327C27C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E1AB19-E45E-429B-81F6-58F4C0011672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-100" yWindow="-100" windowWidth="22378" windowHeight="13337" xr2:uid="{22D8A7BE-9622-49EC-BC9C-1793CE193924}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>Hóa Đơn Bán Hàng</t>
   </si>
@@ -51,40 +51,68 @@
     <t>Thành tiền</t>
   </si>
   <si>
-    <t>Thành Tiền:</t>
-  </si>
-  <si>
     <t>bàn phím gaming</t>
   </si>
   <si>
-    <t>150000.00</t>
-  </si>
-  <si>
     <t>tai nghe gaming</t>
   </si>
   <si>
-    <t>Nguyen thanh huy</t>
-  </si>
-  <si>
-    <t>2023-07-03</t>
-  </si>
-  <si>
-    <t>1350000.00</t>
-  </si>
-  <si>
-    <t>900000.00</t>
-  </si>
-  <si>
-    <t>2100000.00</t>
+    <t>Nguyen thanh tuan</t>
+  </si>
+  <si>
+    <t>2023-05-20</t>
+  </si>
+  <si>
+    <t>Tổng Tiền:</t>
+  </si>
+  <si>
+    <t>20000000.0000000000</t>
+  </si>
+  <si>
+    <t>laptop asus</t>
+  </si>
+  <si>
+    <t>300000.0000000000</t>
+  </si>
+  <si>
+    <t>200000.0000000000</t>
+  </si>
+  <si>
+    <t>tai nghe chụp tai</t>
+  </si>
+  <si>
+    <t>180000.0000000000</t>
+  </si>
+  <si>
+    <t>21650000.0000000000</t>
+  </si>
+  <si>
+    <t>1850000.0000000000</t>
+  </si>
+  <si>
+    <t>250000.0000000000</t>
+  </si>
+  <si>
+    <t>1960000.0000000000</t>
+  </si>
+  <si>
+    <t>900000.0000000000</t>
   </si>
   <si>
     <t>chuột gaming</t>
+  </si>
+  <si>
+    <t>700000.0000000000</t>
+  </si>
+  <si>
+    <t>chuột không dây</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -122,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -133,6 +161,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -451,18 +482,18 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.46484375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.53125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.3203125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.25"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="7.88671875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.41796875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="19.43359375"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
@@ -503,27 +534,27 @@
       <c r="E5" s="4"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="B8">
-        <v>128</v>
+      <c r="B8" t="n" s="0">
+        <v>1140.0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
-        <v>13</v>
+      <c r="B9" t="s" s="0">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B10" t="s">
-        <v>12</v>
+      <c r="B10" t="s" s="0">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
@@ -541,50 +572,63 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B15" t="s">
+      <c r="B15" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C15" t="n" s="0">
+        <v>900000.0</v>
+      </c>
+      <c r="D15" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="E15" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="G15" s="0"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B16" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="C16" t="n" s="0">
+        <v>700000.0</v>
+      </c>
+      <c r="D16" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="E16" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G16" s="0"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B17" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C17" t="n" s="0">
+        <v>200000.0</v>
+      </c>
+      <c r="D17" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="E17" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="G17" s="0"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B18" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C15">
-        <v>300000</v>
-      </c>
-      <c r="D15">
-        <v>3</v>
-      </c>
-      <c r="E15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16">
-        <v>700000</v>
-      </c>
-      <c r="D16">
-        <v>3</v>
-      </c>
-      <c r="E16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17">
-        <v>150000</v>
-      </c>
-      <c r="D17">
+      <c r="C18" s="0">
+        <v>180000</v>
+      </c>
+      <c r="D18" s="0">
         <v>1</v>
       </c>
-      <c r="E17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="C18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="E18" t="s" s="0">
+        <v>18</v>
+      </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.45">
       <c r="C19" s="2"/>
@@ -623,11 +667,11 @@
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="F28" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28" t="s">
-        <v>14</v>
+      <c r="F28" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="G28" t="s" s="0">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>